<commit_message>
Table Validation hopefully done & challan need to be Implement
</commit_message>
<xml_diff>
--- a/Invoiceasy/Libs/Files/CoreFiles/TemplateFiles/invoice-template.xlsx
+++ b/Invoiceasy/Libs/Files/CoreFiles/TemplateFiles/invoice-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzsmu\source\repos\EasyInvoice\EasyInvoice\bin\Debug\netcoreapp3.0\Libs\Files\CoreFiles\TemplateFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzsmu\source\repos\Invoiceasy\Invoiceasy\Libs\Files\CoreFiles\TemplateFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B562495-5AB8-41F1-BC8A-43931CA01D6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09462CB5-6595-4FE2-9566-073919CEF184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,6 +493,48 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -519,48 +561,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,30 +1244,30 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
     </row>
     <row r="4" spans="1:7" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
     </row>
     <row r="5" spans="1:7" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1278,7 +1278,7 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="57" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="7"/>
@@ -1289,64 +1289,64 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44" t="s">
+      <c r="A7" s="57"/>
+      <c r="B7" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
     </row>
     <row r="8" spans="1:7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
       <c r="F8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" customFormat="1" ht="31.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
     </row>
     <row r="11" spans="1:7" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
     </row>
     <row r="12" spans="1:7" s="15" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
@@ -1365,31 +1365,25 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
       <c r="F13" s="24"/>
-      <c r="G13" s="25">
-        <f>F13*E13</f>
-        <v>0</v>
-      </c>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
       <c r="F14" s="24"/>
-      <c r="G14" s="25">
-        <f t="shared" ref="G14:G36" si="0">F14*E14</f>
-        <v>0</v>
-      </c>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="20"/>
@@ -1397,133 +1391,100 @@
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
       <c r="F16" s="26"/>
-      <c r="G16" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
       <c r="F17" s="24"/>
-      <c r="G17" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
       <c r="F18" s="24"/>
-      <c r="G18" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
       <c r="D19" s="22"/>
       <c r="E19" s="25"/>
       <c r="F19" s="27"/>
-      <c r="G19" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="20"/>
       <c r="C20" s="28"/>
       <c r="D20" s="22"/>
       <c r="E20" s="25"/>
       <c r="F20" s="27"/>
-      <c r="G20" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="20"/>
       <c r="C21" s="28"/>
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
       <c r="F21" s="27"/>
-      <c r="G21" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="20"/>
       <c r="C22" s="28"/>
       <c r="D22" s="22"/>
       <c r="E22" s="25"/>
       <c r="F22" s="27"/>
-      <c r="G22" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="20"/>
       <c r="C23" s="28"/>
       <c r="D23" s="22"/>
       <c r="E23" s="25"/>
       <c r="F23" s="27"/>
-      <c r="G23" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="20"/>
       <c r="C24" s="28"/>
       <c r="D24" s="22"/>
       <c r="E24" s="25"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="20"/>
       <c r="C25" s="28"/>
       <c r="D25" s="22"/>
       <c r="E25" s="25"/>
       <c r="F25" s="27"/>
-      <c r="G25" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="20"/>
@@ -1531,121 +1492,91 @@
       <c r="D26" s="22"/>
       <c r="E26" s="25"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="20"/>
       <c r="C27" s="28"/>
       <c r="D27" s="22"/>
       <c r="E27" s="25"/>
       <c r="F27" s="27"/>
-      <c r="G27" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="20"/>
       <c r="C28" s="28"/>
       <c r="D28" s="22"/>
       <c r="E28" s="25"/>
       <c r="F28" s="27"/>
-      <c r="G28" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="20"/>
       <c r="C29" s="28"/>
       <c r="D29" s="22"/>
       <c r="E29" s="25"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="20"/>
       <c r="C30" s="28"/>
       <c r="D30" s="22"/>
       <c r="E30" s="25"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="20"/>
       <c r="C31" s="28"/>
       <c r="D31" s="22"/>
       <c r="E31" s="25"/>
       <c r="F31" s="27"/>
-      <c r="G31" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G31" s="25"/>
     </row>
     <row r="32" spans="1:7" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="20"/>
       <c r="C32" s="28"/>
       <c r="D32" s="29"/>
       <c r="E32" s="25"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="1:11" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="20"/>
       <c r="C33" s="28"/>
       <c r="D33" s="29"/>
       <c r="E33" s="13"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="1:11" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="20"/>
       <c r="C34" s="28"/>
       <c r="D34" s="29"/>
       <c r="E34" s="13"/>
       <c r="F34" s="27"/>
-      <c r="G34" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="1:11" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="13"/>
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="13"/>
       <c r="F35" s="30"/>
-      <c r="G35" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G35" s="25"/>
     </row>
     <row r="36" spans="1:11" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="13"/>
       <c r="C36" s="29"/>
       <c r="D36" s="29" t="s">
@@ -1653,37 +1584,28 @@
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="30"/>
-      <c r="G36" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="1:11" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="13"/>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
       <c r="E37" s="13"/>
       <c r="F37" s="30"/>
-      <c r="G37" s="25">
-        <f>F37*E37</f>
-        <v>0</v>
-      </c>
+      <c r="G37" s="25"/>
     </row>
     <row r="38" spans="1:11" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="13"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
       <c r="E38" s="13"/>
       <c r="F38" s="30"/>
-      <c r="G38" s="25">
-        <f>F38*E38</f>
-        <v>0</v>
-      </c>
+      <c r="G38" s="25"/>
     </row>
     <row r="39" spans="1:11" s="15" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="45" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="13"/>
@@ -1691,68 +1613,56 @@
       <c r="D39" s="29"/>
       <c r="E39" s="31"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="25">
-        <f t="shared" ref="G39" si="1">F39*E39</f>
-        <v>0</v>
-      </c>
+      <c r="G39" s="25"/>
     </row>
     <row r="40" spans="1:11" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
-      <c r="B40" s="56" t="s">
+      <c r="A40" s="45"/>
+      <c r="B40" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="57" t="s">
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="57"/>
-      <c r="G40" s="33">
-        <f>SUM(G13:G39)</f>
-        <v>0</v>
-      </c>
+      <c r="F40" s="48"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:11" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="58" t="s">
+      <c r="A41" s="45"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="58"/>
-      <c r="G41" s="25">
-        <f>G40*0.29</f>
-        <v>0</v>
-      </c>
+      <c r="F41" s="49"/>
+      <c r="G41" s="25"/>
     </row>
     <row r="42" spans="1:11" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="59" t="s">
+      <c r="A42" s="45"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="F42" s="59"/>
-      <c r="G42" s="25">
-        <f>G40-G41</f>
-        <v>0</v>
-      </c>
+      <c r="F42" s="50"/>
+      <c r="G42" s="25"/>
     </row>
     <row r="43" spans="1:11" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
+      <c r="A43" s="45"/>
       <c r="B43" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="60"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
     </row>
     <row r="44" spans="1:11" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
+      <c r="A44" s="45"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
       <c r="D44" s="16"/>
@@ -1761,32 +1671,32 @@
       <c r="G44" s="36"/>
     </row>
     <row r="45" spans="1:11" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
+      <c r="A45" s="45"/>
       <c r="B45" s="37"/>
       <c r="C45" s="37"/>
       <c r="D45" s="16"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
     </row>
     <row r="46" spans="1:11" s="15" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
-      <c r="B46" s="49" t="s">
+      <c r="A46" s="45"/>
+      <c r="B46" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="49"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="16"/>
       <c r="E46" s="35"/>
-      <c r="F46" s="49" t="s">
+      <c r="F46" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="49"/>
+      <c r="G46" s="40"/>
       <c r="K46" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="55"/>
+      <c r="A47" s="46"/>
       <c r="B47" s="16"/>
       <c r="C47" s="38"/>
       <c r="D47" s="39"/>
@@ -1795,18 +1705,26 @@
       <c r="G47" s="36"/>
     </row>
     <row r="48" spans="1:11" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="50" t="s">
+      <c r="A48" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="F46:G46"/>
     <mergeCell ref="A48:G48"/>
     <mergeCell ref="A15:A25"/>
@@ -1819,14 +1737,6 @@
     <mergeCell ref="C43:G43"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="E2:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="92" orientation="portrait" r:id="rId1"/>

</xml_diff>